<commit_message>
excel import command happy flow working
</commit_message>
<xml_diff>
--- a/backend/Pubquiz.Domain.Tests/testfiles/PeCe.xlsx
+++ b/backend/Pubquiz.Domain.Tests/testfiles/PeCe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\pubquiz\backend\Pubquiz.Domain.Tests\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604AF6A5-D263-4085-9DE4-4B860AB7DF60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B66A49-C584-418E-84DE-160FA2B48AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{A6F7848D-7C4F-FD4F-B564-0185C49679BC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>Titel</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Wat is de naam van de droogste champagnesoort?</t>
   </si>
   <si>
-    <t>Sec</t>
-  </si>
-  <si>
     <t>Hoe heet de schrijver van ‘The Hitchhiker's Guide to the Galaxy’?</t>
   </si>
   <si>
@@ -190,15 +187,9 @@
     <t>Choices</t>
   </si>
   <si>
-    <t>Brut;Sec;Doux</t>
-  </si>
-  <si>
     <t>Vanalles 2 - 2</t>
   </si>
   <si>
-    <t>Douglas Adams;Adams</t>
-  </si>
-  <si>
     <t>MediaTitle</t>
   </si>
   <si>
@@ -233,9 +224,6 @@
   </si>
   <si>
     <t>Hoe heet de componist?</t>
-  </si>
-  <si>
-    <t>Brahms;Johannes Brahms</t>
   </si>
   <si>
     <t>Vanalles 1 - 4</t>
@@ -259,6 +247,15 @@
   </si>
   <si>
     <t>MediaFileName</t>
+  </si>
+  <si>
+    <t>Brut||Sec||Doux</t>
+  </si>
+  <si>
+    <t>Brahms&amp;&amp;Johannes Brahms</t>
+  </si>
+  <si>
+    <t>Douglas Adams&amp;&amp;Adams</t>
   </si>
 </sst>
 </file>
@@ -694,10 +691,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +708,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="M10" sqref="M10:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -728,105 +725,105 @@
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="O1" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="7" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="8"/>
       <c r="F2" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:16" s="7" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
@@ -835,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>4</v>
@@ -843,19 +840,22 @@
       <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
-        <v>42</v>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -864,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>3</v>
@@ -872,28 +872,31 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
-        <v>44</v>
+      <c r="N5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
@@ -901,16 +904,19 @@
       <c r="L6">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
-        <v>47</v>
+      <c r="N6" t="s">
+        <v>46</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
+      <c r="P6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>7</v>
@@ -918,60 +924,66 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>6</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
+      <c r="P7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="J8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" s="7">
-        <v>1</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>66</v>
+      <c r="O8" s="7">
+        <v>0</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -980,74 +992,77 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>9</v>
-      </c>
-      <c r="N9" t="s">
-        <v>51</v>
+        <v>70</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="L10">
         <v>1</v>
       </c>
-      <c r="M10" t="s">
-        <v>53</v>
+      <c r="N10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>0</v>
@@ -1055,45 +1070,54 @@
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11" t="s">
-        <v>14</v>
+      <c r="N11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
-      <c r="M12" t="s">
-        <v>15</v>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
       </c>
       <c r="P12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
-      <c r="M13" t="s">
-        <v>16</v>
+      <c r="N13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
       </c>
       <c r="P13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1101,7 +1125,7 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E1802D06-D895-FA4F-988E-42A775C2771D}">
           <x14:formula1>
             <xm:f>Lookups!$A$2:$A$7</xm:f>
@@ -1142,70 +1166,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1"/>
     </row>

</xml_diff>